<commit_message>
modified build.gradle to accept environment vriables
</commit_message>
<xml_diff>
--- a/src/main/resources/ConfigAndTestData.xlsx
+++ b/src/main/resources/ConfigAndTestData.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="SignUpTests" sheetId="3" r:id="rId1"/>
-    <sheet name="signUpUserTest" sheetId="1" r:id="rId2"/>
-    <sheet name="updateProfileTest" sheetId="2" r:id="rId3"/>
+    <sheet name="signUpUserTest" sheetId="1" r:id="rId1"/>
+    <sheet name="updateProfileTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="53">
   <si>
     <t>Active</t>
   </si>
@@ -132,12 +131,6 @@
     <t>firefox</t>
   </si>
   <si>
-    <t>49.0</t>
-  </si>
-  <si>
-    <t>Windows 7</t>
-  </si>
-  <si>
     <t>safari</t>
   </si>
   <si>
@@ -145,6 +138,42 @@
   </si>
   <si>
     <t>10.0</t>
+  </si>
+  <si>
+    <t>MicrosoftEdge</t>
+  </si>
+  <si>
+    <t>14.14393</t>
+  </si>
+  <si>
+    <t>OS X 10.10</t>
+  </si>
+  <si>
+    <t>54.0</t>
+  </si>
+  <si>
+    <t>55.0</t>
+  </si>
+  <si>
+    <t>Test04</t>
+  </si>
+  <si>
+    <t>Test05</t>
+  </si>
+  <si>
+    <t>test07@gmail.com</t>
+  </si>
+  <si>
+    <t>test08@gmail.com</t>
+  </si>
+  <si>
+    <t>test09@gmail.com</t>
+  </si>
+  <si>
+    <t>test10@gmail.com</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
@@ -174,7 +203,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,6 +219,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,14 +256,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -535,178 +576,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B2:B4" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3">
+      <c r="G2" s="3">
         <v>12345678</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
+      <c r="G3" s="3">
         <v>12345678</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="3">
+      <c r="G4" s="3">
         <v>12345678</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" s="3" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="3">
+        <v>12345678</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="3">
+        <v>12345678</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -714,214 +791,365 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="2" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3">
+      <c r="G2" s="3">
         <v>12345678</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>12345</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3">
+        <v>12345678</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>12346</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3">
+        <v>12345678</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>12347</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="3">
+        <v>12345678</v>
+      </c>
+      <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="J5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="3">
-        <v>12345</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q5" s="3">
+        <v>12347</v>
+      </c>
+      <c r="R5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="F6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="3">
         <v>12345678</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="H6" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I6" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="3" t="s">
+      <c r="J6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="3">
-        <v>12346</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3">
-        <v>12345678</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="3">
+      <c r="Q6" s="3">
         <v>12347</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>